<commit_message>
get instructor and user info of instructor home page
</commit_message>
<xml_diff>
--- a/docAPI.xlsx
+++ b/docAPI.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="21">
   <si>
     <t>title</t>
   </si>
@@ -75,6 +75,18 @@
   </si>
   <si>
     <t>get courses by category</t>
+  </si>
+  <si>
+    <t>Course</t>
+  </si>
+  <si>
+    <t>/courses</t>
+  </si>
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>get courses detail by id</t>
   </si>
 </sst>
 </file>
@@ -408,10 +420,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I3"/>
+  <dimension ref="A1:I4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -486,6 +498,23 @@
         <v>16</v>
       </c>
     </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" t="s">
+        <v>18</v>
+      </c>
+      <c r="E4" t="s">
+        <v>19</v>
+      </c>
+      <c r="G4" t="s">
+        <v>20</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
update doc, hash password
</commit_message>
<xml_diff>
--- a/docAPI.xlsx
+++ b/docAPI.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="32">
   <si>
     <t>title</t>
   </si>
@@ -87,6 +87,78 @@
   </si>
   <si>
     <t>get courses detail by id</t>
+  </si>
+  <si>
+    <t>Authentication</t>
+  </si>
+  <si>
+    <t>post</t>
+  </si>
+  <si>
+    <t>/authentication</t>
+  </si>
+  <si>
+    <t>email, password</t>
+  </si>
+  <si>
+    <t>login</t>
+  </si>
+  <si>
+    <t>token, user info</t>
+  </si>
+  <si>
+    <t>/signup</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">email, password, name, type (Instructor, Administrator, Student) </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(not null)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">first_name, last_name, gender, birthday, avatar_url, user_address </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(option)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">if type is Instructor: job_title, short_description, full_description </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(option)</t>
+    </r>
+  </si>
+  <si>
+    <t>signup</t>
   </si>
 </sst>
 </file>
@@ -420,22 +492,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I4"/>
+  <dimension ref="A1:I8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="8" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="65.85546875" customWidth="1"/>
+    <col min="6" max="6" width="68.85546875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="63.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
@@ -515,6 +587,50 @@
         <v>20</v>
       </c>
     </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C5" t="s">
+        <v>23</v>
+      </c>
+      <c r="F5" t="s">
+        <v>24</v>
+      </c>
+      <c r="G5" t="s">
+        <v>25</v>
+      </c>
+      <c r="H5" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>22</v>
+      </c>
+      <c r="C6" t="s">
+        <v>27</v>
+      </c>
+      <c r="F6" t="s">
+        <v>28</v>
+      </c>
+      <c r="G6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F7" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F8" t="s">
+        <v>30</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>